<commit_message>
Organizing QB website 1/7
</commit_message>
<xml_diff>
--- a/Data/RISERCC.xlsx
+++ b/Data/RISERCC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Question</t>
   </si>
@@ -82,7 +82,7 @@
     </r>
   </si>
   <si>
-    <t>15, 34, 38</t>
+    <t>15, 34, 38. 42</t>
   </si>
   <si>
     <t>Since the coronavirus (COVID-19) pandemic, for the following questions, please indicate how often you were concerned about the following regarding your child(ren) between the ages of 0-5.
@@ -97,7 +97,7 @@
 • Being treated unfairly by other children</t>
   </si>
   <si>
-    <t>15. 34, 38</t>
+    <t>15. 34, 38, 42</t>
   </si>
   <si>
     <t>Please indicate whether you have experienced any of the following prior to the coronavirus (COVID-19) pandemic
@@ -133,6 +133,9 @@
       </rPr>
       <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2643465/</t>
     </r>
+  </si>
+  <si>
+    <t>15, 34, 38, 42</t>
   </si>
   <si>
     <t>Please indicate whether you have experienced any of the following since the coronavirus (COVID-19) pandemic
@@ -1413,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1"/>
@@ -1492,12 +1495,12 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="372" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -1509,41 +1512,41 @@
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="170.1" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="170.1" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1">

</xml_diff>